<commit_message>
Updating refer a friend func
</commit_message>
<xml_diff>
--- a/SVCareers_Automation_Testing_Project/Data/ReferFriend.xlsx
+++ b/SVCareers_Automation_Testing_Project/Data/ReferFriend.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="32">
   <si>
     <t>UserName</t>
   </si>
@@ -74,43 +74,52 @@
     <t>Washington</t>
   </si>
   <si>
+    <t>.Net</t>
+  </si>
+  <si>
+    <t>Candidate has H1B visa</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>CandidateType</t>
+  </si>
+  <si>
+    <t>ExperienceInYrs</t>
+  </si>
+  <si>
+    <t>NoticePeriodInDays</t>
+  </si>
+  <si>
+    <t>C:\\Work\\Resume.pdf</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>SearchKeyword</t>
+  </si>
+  <si>
+    <t>Fresher</t>
+  </si>
+  <si>
+    <t>George.Thompson2@gmail.com8888888888</t>
+  </si>
+  <si>
     <t>Experienced</t>
   </si>
   <si>
-    <t>.Net</t>
-  </si>
-  <si>
-    <t>Candidate has H1B visa</t>
-  </si>
-  <si>
-    <t>male</t>
-  </si>
-  <si>
-    <t>CandidateType</t>
-  </si>
-  <si>
-    <t>ExperienceInYrs</t>
-  </si>
-  <si>
-    <t>NoticePeriodInDays</t>
-  </si>
-  <si>
-    <t>C:\\Work\\Resume.pdf</t>
-  </si>
-  <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>Testing</t>
-  </si>
-  <si>
-    <t>India</t>
-  </si>
-  <si>
-    <t>SearchKeyword</t>
-  </si>
-  <si>
-    <t>George.Thompson1@gmail.com</t>
+    <t>Available for immediate joining</t>
+  </si>
+  <si>
+    <t>George.Thompson1a973@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -481,7 +490,7 @@
   <dimension ref="A1:P4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,16 +537,16 @@
         <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="2" t="s">
         <v>20</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>8</v>
@@ -546,10 +555,10 @@
         <v>9</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:16" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -569,45 +578,88 @@
         <v>14</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H2" s="3">
-        <v>9999999989</v>
+        <v>3333333333</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="J2" s="3">
         <v>5</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="L2" s="3">
         <v>60</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="N2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="O2" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="P2" s="5" t="s">
+      <c r="G3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H3" s="3">
+        <v>8788888888</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="5" t="s">
         <v>25</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
+    <hyperlink ref="G3" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>